<commit_message>
Alpha 1.3 With ODM modifications
</commit_message>
<xml_diff>
--- a/IBMContractNotifier/FilterRules.xlsx
+++ b/IBMContractNotifier/FilterRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ibmcn\ibmcn\ibmcn\IBMContractNotifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2766F-5EFB-4257-96CC-511795A49C27}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15316D5E-045A-4ED2-8E9F-837F837297EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3144" yWindow="1572" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{1CB714F7-3499-46D3-9D64-0E4079AA7CD1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CB714F7-3499-46D3-9D64-0E4079AA7CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Field Name</t>
   </si>
@@ -97,29 +97,14 @@
     <t>comparison type values</t>
   </si>
   <si>
-    <t>Sender Email:</t>
-  </si>
-  <si>
-    <t>Sender Email password:</t>
-  </si>
-  <si>
-    <t>135791113M</t>
-  </si>
-  <si>
     <t>Included values</t>
-  </si>
-  <si>
-    <t>ibmcnsender@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=";;;**"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,27 +120,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,11 +138,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -187,23 +157,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0030F9-E72B-4148-ABA5-5BF7CFC1B7CB}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,13 +493,13 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -650,13 +608,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{465A4A4F-0EC5-4A50-B64D-53A9E70C507A}">
           <x14:formula1>
-            <xm:f>config!$A$5:$A$6</xm:f>
+            <xm:f>config!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66AA54EB-CB7C-4657-ACB6-C586FDE1B824}">
           <x14:formula1>
-            <xm:f>config!$B$5:$B$6</xm:f>
+            <xm:f>config!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -668,10 +626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BC86F6-9BB9-479F-9F33-E01D1435702D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,57 +641,31 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>23</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uLqQ+O3daP7Bt5EhpZFgflt4Advgcujs2UquQ7pnOvzld2oCbWTqdeM8D0LluiGk9yGbm8ViiwQ6lxrIur7X9Q==" saltValue="0qry8+YqDsH3e422Ed8Ukg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="A3:B3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="ibmcmsender@gmail.com" xr:uid="{22C90184-816F-406D-BFC1-3A8A63AFF15A}"/>
-  </hyperlinks>
+  <sheetProtection algorithmName="SHA-512" hashValue="qQ0CTRM/IJE0ml6qO9m+kpAq8x5PPK5uqo/BqevsKlIU5Q1ApAlH38mLSj0f/jHLkpctiHplV7mym/ALLpKRcQ==" saltValue="eWOoSflK5o+qBeQMD+QyiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IBMCN Version 1.0 Cut Off
</commit_message>
<xml_diff>
--- a/IBMContractNotifier/FilterRules.xlsx
+++ b/IBMContractNotifier/FilterRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ibmcn\ibmcn\ibmcn\IBMContractNotifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15316D5E-045A-4ED2-8E9F-837F837297EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678D16EF-FDE7-414A-8D96-027FB33CEDA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CB714F7-3499-46D3-9D64-0E4079AA7CD1}"/>
+    <workbookView xWindow="4188" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{1CB714F7-3499-46D3-9D64-0E4079AA7CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>OppName</t>
   </si>
   <si>
-    <t>sales order</t>
-  </si>
-  <si>
     <t>IMT</t>
   </si>
   <si>
@@ -64,40 +61,43 @@
     <t>AccountID</t>
   </si>
   <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>TCV</t>
+  </si>
+  <si>
+    <t>Div Code</t>
+  </si>
+  <si>
+    <t>SignProbability</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>contain</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>declined</t>
+  </si>
+  <si>
+    <t>comparison type values</t>
+  </si>
+  <si>
+    <t>Included values</t>
+  </si>
+  <si>
+    <t>Sales Order</t>
+  </si>
+  <si>
     <t>TBD</t>
-  </si>
-  <si>
-    <t>Backlog</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>TCV</t>
-  </si>
-  <si>
-    <t>Div Code</t>
-  </si>
-  <si>
-    <t>SignProbability</t>
-  </si>
-  <si>
-    <t>equal</t>
-  </si>
-  <si>
-    <t>contain</t>
-  </si>
-  <si>
-    <t>accepted</t>
-  </si>
-  <si>
-    <t>declined</t>
-  </si>
-  <si>
-    <t>comparison type values</t>
-  </si>
-  <si>
-    <t>Included values</t>
   </si>
 </sst>
 </file>
@@ -505,16 +505,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -523,61 +523,61 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -585,7 +585,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -593,7 +593,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -641,26 +641,26 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>